<commit_message>
further finished, some problem with times in the example sheet
</commit_message>
<xml_diff>
--- a/example/exampledata.xlsx
+++ b/example/exampledata.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="instructions" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="97">
   <si>
     <t xml:space="preserve">Instructions</t>
   </si>
@@ -192,6 +192,9 @@
     <t xml:space="preserve">chair</t>
   </si>
   <si>
+    <t xml:space="preserve">items</t>
+  </si>
+  <si>
     <t xml:space="preserve">Designing for User Engagement</t>
   </si>
   <si>
@@ -256,6 +259,9 @@
   </si>
   <si>
     <t xml:space="preserve">Grand Ballroom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PLENARY</t>
   </si>
   <si>
     <t xml:space="preserve">Paper Session: Surprise and Startle</t>
@@ -329,6 +335,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -357,6 +364,7 @@
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -445,11 +453,11 @@
   </sheetPr>
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A6" activeCellId="1" sqref="D2 A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="125.88"/>
   </cols>
@@ -483,10 +491,10 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D31" activeCellId="0" sqref="D31"/>
+      <selection pane="topLeft" activeCell="D31" activeCellId="1" sqref="D2 D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.99"/>
@@ -804,15 +812,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="45.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.94"/>
   </cols>
@@ -836,25 +844,28 @@
       <c r="F1" s="0" t="s">
         <v>53</v>
       </c>
+      <c r="G1" s="0" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -862,19 +873,19 @@
         <v>9</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -882,19 +893,19 @@
         <v>12</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -902,16 +913,16 @@
         <v>15</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F5" s="0" t="s">
         <v>30</v>
@@ -933,36 +944,39 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
+      <selection pane="topLeft" activeCell="F4" activeCellId="1" sqref="D2 F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="61.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="61.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.2"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D1" s="0" t="s">
         <v>5</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F1" s="0" t="s">
         <v>51</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -976,10 +990,13 @@
         <v>0.4375</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -993,13 +1010,13 @@
         <v>0.479166666666667</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1013,13 +1030,13 @@
         <v>0.520833333333333</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1033,13 +1050,13 @@
         <v>0.479166666666667</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1053,13 +1070,16 @@
         <v>0.604166666666667</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1101,12 +1121,12 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="1" sqref="D2 C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.14"/>
@@ -1116,42 +1136,42 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
example is functional now
</commit_message>
<xml_diff>
--- a/example/exampledata.xlsx
+++ b/example/exampledata.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="instructions" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,16 +24,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="97">
   <si>
     <t xml:space="preserve">Instructions</t>
   </si>
   <si>
     <t xml:space="preserve">I wrote a program to pick and merge the paper/poster data, time schedule, session organisation from a file with four spreadsheets. 
-- items: This one lists all submitted papers, posters, and panel contributions. The column 'session' indicates where an item will be assigned / grouped.
+- items: This one lists all submitted papers, posters, and panel contributions. The column 'session' indicates where an item will be assigned / grouped. If session does not exist (e.g., ‘REJECTED’), a warning is issued and the item is not included. It is possible to re-use an item for multiple sessions, by giving the session ID’s in a comma separated list.
 - sessions: This just holds the grouping, session titles, chair, etc. The column 'session' has a unique ID for each session, and this ID is used in the items table to link items to sessions. The column 'event' links to the events table that defines schedule/rooms, and defines where in the program the session ends up. It is easy to swap two event ID's around here, to swap two session slots.
-- events: This is essentially the program scheduling. I took Esa's data. Currently all parallel sessions (3 parallel) are fully planned. Don't know how many rooms we have. 
-- authors: This sheet is not strictly needed, authors are extracted from the author_list column in the items, but it can be used to add bios or the like.</t>
+- events: This is essentially the program scheduling. Each event can be assigned a time, a room and optionally a session (a break has no session for example). When multiple events have the same start time, these are seen as parallel.
+- authors: This sheet is not strictly needed, authors are extracted from the author_list column in the items, but it can be used to add bios or the like.
+The authors in the ‘author_list’ field may be separated by commas or by newlines. Common titles (prefix like prof. or postfix like PhD) are recognized, Initials and names are also recognized. So “E. Sarah Wilson, PhD” will be written as Sarah Wilson in the author list under a paper, and in full in the author index (Wilson, E. Sarah, PhD)</t>
   </si>
   <si>
     <t xml:space="preserve">item</t>
@@ -48,6 +49,9 @@
     <t xml:space="preserve">title</t>
   </si>
   <si>
+    <t xml:space="preserve">abstract</t>
+  </si>
+  <si>
     <t xml:space="preserve">WORKLOAD</t>
   </si>
   <si>
@@ -228,7 +232,7 @@
     <t xml:space="preserve">NLP Advances</t>
   </si>
   <si>
-    <t xml:space="preserve">Thu-KS</t>
+    <t xml:space="preserve">Tue-KS</t>
   </si>
   <si>
     <t xml:space="preserve">Dr. David Lee</t>
@@ -268,9 +272,6 @@
   </si>
   <si>
     <t xml:space="preserve">Meeting Room 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tue-KS</t>
   </si>
   <si>
     <t xml:space="preserve">Panel Discussion: The Future of Human-Machine Interaction</t>
@@ -453,11 +454,11 @@
   </sheetPr>
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="1" sqref="D2 A6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="125.88"/>
   </cols>
@@ -467,7 +468,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="202.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -488,13 +489,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D31" activeCellId="1" sqref="D2 D31"/>
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.99"/>
@@ -515,19 +516,22 @@
       <c r="D1" s="0" t="s">
         <v>5</v>
       </c>
+      <c r="E1" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -535,13 +539,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -549,13 +553,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -563,13 +567,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -577,13 +581,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -591,13 +595,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -605,13 +609,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -619,13 +623,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -633,13 +637,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -647,13 +651,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -661,13 +665,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -675,13 +679,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -689,13 +693,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -703,13 +707,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -717,13 +721,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -731,13 +735,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -745,13 +749,13 @@
         <v>17</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -759,13 +763,13 @@
         <v>18</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -773,13 +777,13 @@
         <v>19</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -787,13 +791,13 @@
         <v>20</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -814,13 +818,13 @@
   </sheetPr>
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="45.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.94"/>
   </cols>
@@ -833,99 +837,99 @@
         <v>5</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -944,13 +948,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F4" activeCellId="1" sqref="D2 F4"/>
+      <selection pane="topLeft" activeCell="H34" activeCellId="0" sqref="H34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="61.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.2"/>
@@ -958,25 +962,25 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D1" s="0" t="s">
         <v>5</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -990,13 +994,13 @@
         <v>0.4375</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1010,13 +1014,13 @@
         <v>0.479166666666667</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1036,7 +1040,7 @@
         <v>82</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1053,10 +1057,10 @@
         <v>83</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1073,34 +1077,14 @@
         <v>84</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
+        <v>78</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1121,10 +1105,10 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="1" sqref="D2 C3"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.14"/>

</xml_diff>